<commit_message>
replacing files with master branch files
</commit_message>
<xml_diff>
--- a/mobile/src/main/resources/Config.xlsx
+++ b/mobile/src/main/resources/Config.xlsx
@@ -56,10 +56,10 @@
     <t>Sanity.xlsx</t>
   </si>
   <si>
-    <t>test2</t>
-  </si>
-  <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>wild1</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,13 +428,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>

</xml_diff>